<commit_message>
moved the file structure
</commit_message>
<xml_diff>
--- a/Utils/Data/deals_data_model.xlsx
+++ b/Utils/Data/deals_data_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Admin/Documents/GitHub/banner_magic/Utils/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2490FAE7-98BD-B644-B206-43BBA1ADBB58}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B31C846-8F1E-B246-B328-EA60B345FD39}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24340" yWindow="-21140" windowWidth="37620" windowHeight="19420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26420" yWindow="-19180" windowWidth="37620" windowHeight="19420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>Astracast Granite</t>
   </si>
@@ -54,9 +54,6 @@
     <t>YES</t>
   </si>
   <si>
-    <t>warranty</t>
-  </si>
-  <si>
     <t>NO</t>
   </si>
   <si>
@@ -85,9 +82,6 @@
   </si>
   <si>
     <t>PROMO TEXT LINE 1</t>
-  </si>
-  <si>
-    <t>PROMO TEXT LINE 2</t>
   </si>
   <si>
     <t>URL LINK</t>
@@ -463,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -481,55 +475,52 @@
     <col min="9" max="9" width="31.1640625" style="3" customWidth="1"/>
     <col min="10" max="10" width="28.1640625" customWidth="1"/>
     <col min="11" max="11" width="21.83203125" customWidth="1"/>
-    <col min="12" max="13" width="22" customWidth="1"/>
-    <col min="14" max="14" width="31.6640625" customWidth="1"/>
+    <col min="12" max="12" width="22" customWidth="1"/>
+    <col min="13" max="13" width="31.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>21</v>
-      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -543,7 +534,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>6</v>
@@ -557,21 +548,18 @@
         <v>8</v>
       </c>
       <c r="K2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>30</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>32</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -583,28 +571,28 @@
         <v>7</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M3" t="s">
-        <v>28</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>23</v>
+        <v>9</v>
+      </c>
+      <c r="L3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added in some more hp banner logic for deals
</commit_message>
<xml_diff>
--- a/Utils/Data/deals_data_model.xlsx
+++ b/Utils/Data/deals_data_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Admin/Documents/GitHub/banner_magic/Utils/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B31C846-8F1E-B246-B328-EA60B345FD39}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA8088FB-5807-544F-9D01-A0E00C2D940E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26420" yWindow="-19180" windowWidth="37620" windowHeight="19420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25880" yWindow="-20480" windowWidth="37620" windowHeight="19420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
   <si>
     <t>Astracast Granite</t>
   </si>
@@ -69,9 +69,6 @@
     <t>NOW PRICE</t>
   </si>
   <si>
-    <t>IMAGE LINK</t>
-  </si>
-  <si>
     <t>MESSAGE TWO LINE 1</t>
   </si>
   <si>
@@ -121,6 +118,18 @@
   </si>
   <si>
     <t>35%</t>
+  </si>
+  <si>
+    <t>CAT IMAGE LINK</t>
+  </si>
+  <si>
+    <t>HP IMAGE LINK</t>
+  </si>
+  <si>
+    <t>https://via.placeholder.com/500x50</t>
+  </si>
+  <si>
+    <t>HP</t>
   </si>
 </sst>
 </file>
@@ -457,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L1048576"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -470,18 +479,19 @@
     <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.83203125" customWidth="1"/>
     <col min="6" max="6" width="32.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.83203125" customWidth="1"/>
-    <col min="8" max="8" width="30.5" customWidth="1"/>
-    <col min="9" max="9" width="31.1640625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="28.1640625" customWidth="1"/>
-    <col min="11" max="11" width="21.83203125" customWidth="1"/>
-    <col min="12" max="12" width="22" customWidth="1"/>
-    <col min="13" max="13" width="31.6640625" customWidth="1"/>
+    <col min="7" max="7" width="32.1640625" customWidth="1"/>
+    <col min="8" max="8" width="18.83203125" customWidth="1"/>
+    <col min="9" max="9" width="30.5" customWidth="1"/>
+    <col min="10" max="10" width="31.1640625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="28.1640625" customWidth="1"/>
+    <col min="12" max="12" width="21.83203125" customWidth="1"/>
+    <col min="13" max="13" width="22" customWidth="1"/>
+    <col min="14" max="14" width="31.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>10</v>
@@ -496,31 +506,37 @@
         <v>13</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="K1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>19</v>
+      <c r="O1" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -534,32 +550,38 @@
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="1" t="s">
+      <c r="I2" s="1"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>27</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -571,28 +593,34 @@
         <v>7</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L3" t="s">
-        <v>26</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>21</v>
+      <c r="M3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new deals lsh template
</commit_message>
<xml_diff>
--- a/Utils/Data/deals_data_model.xlsx
+++ b/Utils/Data/deals_data_model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11109"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Admin/Documents/GitHub/banner_magic/Utils/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Admin/Documents/Applications/banner_magic/Utils/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF142470-0F78-FC40-B40E-51149D472F58}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6710B3B-1CD0-004B-90E6-145A60C7B7DC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13500" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15180" yWindow="-20260" windowWidth="34960" windowHeight="20080" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,32 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
-  <si>
-    <t>Astracast Granite</t>
-  </si>
-  <si>
-    <t>Was from £125.99</t>
-  </si>
-  <si>
-    <t>Sinks</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="82">
   <si>
     <t>Save over</t>
   </si>
   <si>
-    <t>This is a new</t>
-  </si>
-  <si>
-    <t>Line of text</t>
-  </si>
-  <si>
-    <t>https://via.placeholder.com/135x135</t>
-  </si>
-  <si>
-    <t>Was £56.99</t>
-  </si>
-  <si>
     <t>YES</t>
   </si>
   <si>
@@ -84,59 +63,221 @@
     <t>URL LINK</t>
   </si>
   <si>
-    <t>https://www.google.co.uk</t>
-  </si>
-  <si>
-    <t>https://www.yahoo.co.uk</t>
-  </si>
-  <si>
     <t>GENERIC MESSAGE</t>
   </si>
   <si>
-    <t>£80.00</t>
-  </si>
-  <si>
-    <t>£45.00</t>
-  </si>
-  <si>
     <t>PRODUCT CODE</t>
   </si>
   <si>
-    <t>51235F3</t>
-  </si>
-  <si>
-    <t>33434FF</t>
-  </si>
-  <si>
-    <t>100 years</t>
-  </si>
-  <si>
     <t>CATEGORY</t>
   </si>
   <si>
     <t>Bathrooms</t>
   </si>
   <si>
-    <t>35%</t>
-  </si>
-  <si>
     <t>CAT IMAGE LINK</t>
   </si>
   <si>
     <t>HP IMAGE LINK</t>
   </si>
   <si>
-    <t>https://via.placeholder.com/500x50</t>
-  </si>
-  <si>
     <t>HP</t>
+  </si>
+  <si>
+    <t>From</t>
+  </si>
+  <si>
+    <t>£149.00</t>
+  </si>
+  <si>
+    <t>Digital Showers</t>
+  </si>
+  <si>
+    <t>Shower Enclosures</t>
+  </si>
+  <si>
+    <t>Mira Mode</t>
+  </si>
+  <si>
+    <t>Bath Screens</t>
+  </si>
+  <si>
+    <t>30%</t>
+  </si>
+  <si>
+    <t>20%</t>
+  </si>
+  <si>
+    <t>Save</t>
+  </si>
+  <si>
+    <t>Electric Showers</t>
+  </si>
+  <si>
+    <t>Mixer Showers</t>
+  </si>
+  <si>
+    <t>Bathroom Taps</t>
+  </si>
+  <si>
+    <t>Shower Pumps</t>
+  </si>
+  <si>
+    <t>Power Tool Accessories</t>
+  </si>
+  <si>
+    <t>Shower Trays</t>
+  </si>
+  <si>
+    <t>ventilation</t>
+  </si>
+  <si>
+    <t>Nabis Arno</t>
+  </si>
+  <si>
+    <t>Bathroom Pack</t>
+  </si>
+  <si>
+    <t>Raptor Power</t>
+  </si>
+  <si>
+    <t>Tool Accessories</t>
+  </si>
+  <si>
+    <t>Coram Optima</t>
+  </si>
+  <si>
+    <t>Pivot Doors</t>
+  </si>
+  <si>
+    <t>Coram Frameless</t>
+  </si>
+  <si>
+    <t>Nabis Shower</t>
+  </si>
+  <si>
+    <t>Vent Axia</t>
+  </si>
+  <si>
+    <t>Extractor Fans</t>
+  </si>
+  <si>
+    <t>Salamander</t>
+  </si>
+  <si>
+    <t>Homeboost Pump</t>
+  </si>
+  <si>
+    <t>Nabis Bathroom</t>
+  </si>
+  <si>
+    <t>Trays</t>
+  </si>
+  <si>
+    <t>Taps</t>
+  </si>
+  <si>
+    <t>Nabis Twin</t>
+  </si>
+  <si>
+    <t>Shower</t>
+  </si>
+  <si>
+    <t>Triton T80</t>
+  </si>
+  <si>
+    <t>Pro Fit</t>
+  </si>
+  <si>
+    <t>/product/triton-t80-pro-fit-electric-shower-85kw/</t>
+  </si>
+  <si>
+    <t>/product/nabis-twin-erd-thermostatic-bar-valve/</t>
+  </si>
+  <si>
+    <t>/webapp/wcs/stores/servlet/CatalogSearchMobileView?searchTerm=bathroomnabistapsgalene</t>
+  </si>
+  <si>
+    <t>/product/salamander-home-boost-mains-pressure-booster-pump/</t>
+  </si>
+  <si>
+    <t>/showering/showers/digital-showers/?facet2=ads_f10022_ntk_cs:Mode&amp;facet1=ads_f10003_ntk_cs:Mira</t>
+  </si>
+  <si>
+    <t>/product/nabis-arno-round-4-piece-pack/</t>
+  </si>
+  <si>
+    <t>/webapp/wcs/stores/servlet/CatalogSearchView?langId=44&amp;pageSize=12&amp;pageView=detailed&amp;catalogId=12001&amp;searchTerm=wukjandealspowertools&amp;categoryId=&amp;storeId=10203&amp;ddkey=https%3AAjaxCatalogSearchView</t>
+  </si>
+  <si>
+    <t>/webapp/wcs/stores/servlet/CatalogSearchView?langId=44&amp;pageSize=12&amp;pageView=detailed&amp;catalogId=12001&amp;searchTerm=wukjandealsenclosurestrays&amp;categoryId=&amp;storeId=10203&amp;ddkey=https%3AAjaxCatalogSearchView</t>
+  </si>
+  <si>
+    <t>/webapp/wcs/stores/servlet/CatalogSearchView?langId=44&amp;pageSize=12&amp;pageView=detailed&amp;catalogId=12001&amp;searchTerm=wukjandealscoram&amp;categoryId=&amp;storeId=10203&amp;ddkey=https%3AAjaxCatalogSearchView</t>
+  </si>
+  <si>
+    <t>/showering/shower-trays/rectangular-shower-trays/?facet1=ads_f10003_ntk_cs:Nabis</t>
+  </si>
+  <si>
+    <t>/webapp/wcs/stores/servlet/CatalogSearchView?langId=44&amp;pageSize=12&amp;pageView=detailed&amp;catalogId=12001&amp;searchTerm=wukjandealsventilation&amp;categoryId=&amp;storeId=10203&amp;ddkey=https%3AAjaxCatalogSearchView</t>
+  </si>
+  <si>
+    <t>50%</t>
+  </si>
+  <si>
+    <t>40%</t>
+  </si>
+  <si>
+    <t>£95.00</t>
+  </si>
+  <si>
+    <t>£29.99</t>
+  </si>
+  <si>
+    <t>£199.00</t>
+  </si>
+  <si>
+    <t>£235.00</t>
+  </si>
+  <si>
+    <t>£154.00</t>
+  </si>
+  <si>
+    <t>£3.99</t>
+  </si>
+  <si>
+    <t>£130.00</t>
+  </si>
+  <si>
+    <t>£50.00</t>
+  </si>
+  <si>
+    <t>£60.00</t>
+  </si>
+  <si>
+    <t>£10.99</t>
+  </si>
+  <si>
+    <t>D80057</t>
+  </si>
+  <si>
+    <t>D01192</t>
+  </si>
+  <si>
+    <t>D00601</t>
+  </si>
+  <si>
+    <t>B61686</t>
+  </si>
+  <si>
+    <t>various</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -151,6 +292,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -179,13 +332,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,159 +623,472 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.83203125" customWidth="1"/>
-    <col min="2" max="3" width="21.5" customWidth="1"/>
+    <col min="2" max="3" width="38.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.83203125" customWidth="1"/>
-    <col min="6" max="6" width="32.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.1640625" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" customWidth="1"/>
     <col min="8" max="8" width="18.83203125" customWidth="1"/>
     <col min="9" max="9" width="30.5" customWidth="1"/>
     <col min="10" max="10" width="31.1640625" style="3" customWidth="1"/>
     <col min="11" max="11" width="28.1640625" customWidth="1"/>
     <col min="12" max="12" width="21.83203125" customWidth="1"/>
-    <col min="13" max="13" width="22" customWidth="1"/>
-    <col min="14" max="14" width="31.6640625" customWidth="1"/>
+    <col min="13" max="13" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="182" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="B2" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="H2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="O2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="5"/>
+      <c r="K3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="O3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="H4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="O4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="B5" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" s="5"/>
+      <c r="K5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="O5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="H6" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="O6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="H7" t="s">
+        <v>1</v>
+      </c>
+      <c r="I7" s="5"/>
+      <c r="K7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="O7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="M1" s="2" t="s">
+      <c r="B8" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="H8" t="s">
+        <v>2</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="O8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="H9" t="s">
+        <v>2</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M9" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="N9" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="O1" s="2" t="s">
+      <c r="B10" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="H10" t="s">
+        <v>2</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M10" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="N10" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="O10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="H11" t="s">
+        <v>2</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="N11" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="O11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B12" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="H12" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M3" t="s">
-        <v>25</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>9</v>
+      <c r="I12" s="5"/>
+      <c r="K12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M12" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="N12" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="O12" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed data from spreadsheets
</commit_message>
<xml_diff>
--- a/Utils/Data/deals_data_model.xlsx
+++ b/Utils/Data/deals_data_model.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11208"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Admin/Documents/Applications/banner_magic/Utils/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Admin/Documents/GitHub/banner_magic/Utils/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6710B3B-1CD0-004B-90E6-145A60C7B7DC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6C6D686-ED3F-C847-A5ED-537F17BD7CA7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15180" yWindow="-20260" windowWidth="34960" windowHeight="20080" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27320" yWindow="-21140" windowWidth="34960" windowHeight="20080" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -25,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="91">
   <si>
     <t>Save over</t>
   </si>
@@ -75,15 +80,6 @@
     <t>Bathrooms</t>
   </si>
   <si>
-    <t>CAT IMAGE LINK</t>
-  </si>
-  <si>
-    <t>HP IMAGE LINK</t>
-  </si>
-  <si>
-    <t>HP</t>
-  </si>
-  <si>
     <t>From</t>
   </si>
   <si>
@@ -271,6 +267,42 @@
   </si>
   <si>
     <t>various</t>
+  </si>
+  <si>
+    <t>IMAGE LINK</t>
+  </si>
+  <si>
+    <t>https://www.wolseley.co.uk/wcsstore/Wolseley/Attachment/Deals/jan-feb/electric-showers-cat-banner-image.png</t>
+  </si>
+  <si>
+    <t>https://www.wolseley.co.uk/wcsstore/Wolseley/Attachment/Deals/jan-feb/nabis-twin-cat-banner-image.png</t>
+  </si>
+  <si>
+    <t>https://www.wolseley.co.uk/wcsstore/Wolseley/Attachment/Deals/jan-feb/nabis-baths-taps-cat-banner-image.png</t>
+  </si>
+  <si>
+    <t>https://www.wolseley.co.uk/wcsstore/Wolseley/Attachment/Deals/jan-feb/shower-pumps-cat-banner-image.png</t>
+  </si>
+  <si>
+    <t>https://www.wolseley.co.uk/wcsstore/Wolseley/Attachment/Deals/jan-feb/digital-showers-cat-banner-image.png</t>
+  </si>
+  <si>
+    <t>https://www.wolseley.co.uk/wcsstore/Wolseley/Attachment/Deals/jan-feb/nabis-arno-cat-banner-image.png</t>
+  </si>
+  <si>
+    <t>https://www.wolseley.co.uk/wcsstore/Wolseley/Attachment/Deals/jan-feb/power-tool-accessories-cat-banner-image.png</t>
+  </si>
+  <si>
+    <t>https://www.wolseley.co.uk/wcsstore/Wolseley/Attachment/Deals/jan-feb/shower-enclosures-cat-banner-image.png</t>
+  </si>
+  <si>
+    <t>https://www.wolseley.co.uk/wcsstore/Wolseley/Attachment/Deals/jan-feb/bath-screens-cat-banner-image.png</t>
+  </si>
+  <si>
+    <t>https://www.wolseley.co.uk/wcsstore/Wolseley/Attachment/Deals/jan-feb/shower-trays-cat-banner-image.png</t>
+  </si>
+  <si>
+    <t>https://www.wolseley.co.uk/wcsstore/Wolseley/Attachment/Deals/jan-feb/ventilation-cat-banner-image.png</t>
   </si>
 </sst>
 </file>
@@ -623,10 +655,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -635,18 +667,17 @@
     <col min="2" max="3" width="38.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.83203125" customWidth="1"/>
-    <col min="6" max="6" width="13.1640625" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" customWidth="1"/>
-    <col min="8" max="8" width="18.83203125" customWidth="1"/>
-    <col min="9" max="9" width="30.5" customWidth="1"/>
-    <col min="10" max="10" width="31.1640625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="28.1640625" customWidth="1"/>
-    <col min="12" max="12" width="21.83203125" customWidth="1"/>
-    <col min="13" max="13" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="182" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="105" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.83203125" customWidth="1"/>
+    <col min="8" max="8" width="30.5" customWidth="1"/>
+    <col min="9" max="9" width="31.1640625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="28.1640625" customWidth="1"/>
+    <col min="11" max="11" width="21.83203125" customWidth="1"/>
+    <col min="12" max="12" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="182" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -663,432 +694,426 @@
         <v>6</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="E2" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" s="2" t="s">
+      <c r="F3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="5"/>
+      <c r="J3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F5" t="s">
+        <v>83</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="5"/>
+      <c r="J5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
         <v>18</v>
       </c>
+      <c r="B6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="F6" t="s">
+        <v>84</v>
+      </c>
+      <c r="G6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>55</v>
+      </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="H2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="O2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I3" s="5"/>
-      <c r="K3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="O3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="H4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="N4" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="O4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="H5" t="s">
-        <v>1</v>
-      </c>
-      <c r="I5" s="5"/>
-      <c r="K5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="N5" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="O5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="H6" t="s">
-        <v>2</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="M6" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="N6" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="O6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F7" t="s">
+        <v>85</v>
+      </c>
+      <c r="G7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H7" s="5"/>
+      <c r="J7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="D8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F8" t="s">
+        <v>86</v>
+      </c>
+      <c r="G8" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="7" t="s">
+      <c r="C9" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F9" t="s">
+        <v>87</v>
+      </c>
+      <c r="G9" t="s">
+        <v>2</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="M9" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="H7" t="s">
+      <c r="F10" t="s">
+        <v>88</v>
+      </c>
+      <c r="G10" t="s">
+        <v>2</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="M10" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="F11" t="s">
+        <v>89</v>
+      </c>
+      <c r="G11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F12" t="s">
+        <v>90</v>
+      </c>
+      <c r="G12" t="s">
         <v>1</v>
       </c>
-      <c r="I7" s="5"/>
-      <c r="K7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="M7" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="N7" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="O7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="H8" t="s">
-        <v>2</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="M8" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="N8" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="O8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="H9" t="s">
-        <v>2</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="M9" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="N9" s="5" t="s">
+      <c r="H12" s="5"/>
+      <c r="J12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="M12" s="5" t="s">
         <v>61</v>
-      </c>
-      <c r="O9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="H10" t="s">
-        <v>2</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="M10" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="N10" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="O10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="H11" t="s">
-        <v>2</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="M11" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="N11" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="O11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="H12" t="s">
-        <v>1</v>
-      </c>
-      <c r="I12" s="5"/>
-      <c r="K12" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="M12" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="N12" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="O12" t="s">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>